<commit_message>
Updated with initial list
</commit_message>
<xml_diff>
--- a/docs/Software Development/NGC_ADS_Software_Baseline.xlsx
+++ b/docs/Software Development/NGC_ADS_Software_Baseline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>Product</t>
   </si>
@@ -47,6 +47,123 @@
   </si>
   <si>
     <t>Modified</t>
+  </si>
+  <si>
+    <t>AngularJS</t>
+  </si>
+  <si>
+    <t>NodeJS</t>
+  </si>
+  <si>
+    <t>Express JS</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>Zabbix</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>0.12.4</t>
+  </si>
+  <si>
+    <t>4.12.4</t>
+  </si>
+  <si>
+    <t>2.4.5</t>
+  </si>
+  <si>
+    <t>Twitter Bootstrap</t>
+  </si>
+  <si>
+    <t>Front end</t>
+  </si>
+  <si>
+    <t>Graphs/Charts</t>
+  </si>
+  <si>
+    <t>Application Server</t>
+  </si>
+  <si>
+    <t>Container</t>
+  </si>
+  <si>
+    <t>Continuous Monitoring</t>
+  </si>
+  <si>
+    <t>Jenkins</t>
+  </si>
+  <si>
+    <t>MVC Web Application Framework for NodeJS</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Continuous Integrated Builds</t>
+  </si>
+  <si>
+    <t>1.4.1</t>
+  </si>
+  <si>
+    <t>0.4.10</t>
+  </si>
+  <si>
+    <t>1.7.0</t>
+  </si>
+  <si>
+    <t>1.9.5</t>
+  </si>
+  <si>
+    <t>AngularJS v1.4.1 -   (c) 2010-2015 Google, Inc. http://angularjs.org  - License: MIT</t>
+  </si>
+  <si>
+    <t>https://nodejs.org</t>
+  </si>
+  <si>
+    <t>3.2.0</t>
+  </si>
+  <si>
+    <t>https://angularjs.org/</t>
+  </si>
+  <si>
+    <t>http://www.zabbix.com/</t>
+  </si>
+  <si>
+    <t>http://getbootstrap.com</t>
+  </si>
+  <si>
+    <t>Copyright 2011-2015 Twitter, Inc. - Licensed under the MIT license</t>
+  </si>
+  <si>
+    <t>http://c3js.org/</t>
+  </si>
+  <si>
+    <t>https://www.docker.com/</t>
+  </si>
+  <si>
+    <t>https://git-scm.com/</t>
+  </si>
+  <si>
+    <t>https://jenkins-ci.org/</t>
+  </si>
+  <si>
+    <t>1.617</t>
+  </si>
+  <si>
+    <t>NPM Install - The Artistic License 2.0 - Copyright (c) 2000-2006, The Perl Foundation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regents of the University of California, Sun Microsystems, Inc., and other parties.  </t>
+  </si>
+  <si>
+    <t>license.terms</t>
   </si>
 </sst>
 </file>
@@ -99,13 +216,13 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -160,12 +277,12 @@
     <tableColumn id="3" name="License" dataDxfId="8"/>
     <tableColumn id="4" name="Source" dataDxfId="7"/>
     <tableColumn id="5" name="License Text" dataDxfId="6"/>
-    <tableColumn id="6" name="Used In" dataDxfId="0"/>
-    <tableColumn id="7" name="Platform" dataDxfId="5"/>
-    <tableColumn id="8" name="Supported" dataDxfId="4"/>
-    <tableColumn id="14" name="Modified" dataDxfId="3"/>
-    <tableColumn id="9" name="Description" dataDxfId="2"/>
-    <tableColumn id="10" name="Comments" dataDxfId="1"/>
+    <tableColumn id="6" name="Used In" dataDxfId="5"/>
+    <tableColumn id="7" name="Platform" dataDxfId="4"/>
+    <tableColumn id="8" name="Supported" dataDxfId="3"/>
+    <tableColumn id="14" name="Modified" dataDxfId="2"/>
+    <tableColumn id="9" name="Description" dataDxfId="1"/>
+    <tableColumn id="10" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -458,20 +575,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:M1048576"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" style="1" customWidth="1"/>
@@ -517,12 +634,157 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C5" s="3"/>
+      <c r="D5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B12" numberStoredAsText="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -530,21 +792,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F38BE9C869A7742B4F5DC1E261FF831" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c81a3dd503577bf2e55e1cf5f361d623">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -658,10 +905,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BAEFC8-5E64-4DBE-91A8-1626A5AF5EB9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7617F739-067F-4308-8E8E-D48E97AC6C80}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -682,17 +952,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7617F739-067F-4308-8E8E-D48E97AC6C80}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BAEFC8-5E64-4DBE-91A8-1626A5AF5EB9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding more js frameworks
</commit_message>
<xml_diff>
--- a/docs/Software Development/NGC_ADS_Software_Baseline.xlsx
+++ b/docs/Software Development/NGC_ADS_Software_Baseline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
   <si>
     <t>Product</t>
   </si>
@@ -236,6 +236,72 @@
   </si>
   <si>
     <t>Front End - Graphs/Charts</t>
+  </si>
+  <si>
+    <t>Jasmine</t>
+  </si>
+  <si>
+    <t>2.3.4</t>
+  </si>
+  <si>
+    <t>https://github.com/jasmine/jasmine/blob/master/MIT.LICENSE</t>
+  </si>
+  <si>
+    <t>http://jasmine.github.io/2.3/introduction.html</t>
+  </si>
+  <si>
+    <t>JavaScript Testing</t>
+  </si>
+  <si>
+    <t>Karma</t>
+  </si>
+  <si>
+    <t>0.12.36</t>
+  </si>
+  <si>
+    <t>https://github.com/karma-runner/karma/blob/master/LICENSE</t>
+  </si>
+  <si>
+    <t>http://karma-runner.github.io/0.12/index.html</t>
+  </si>
+  <si>
+    <t>Karma-Jasmine</t>
+  </si>
+  <si>
+    <t>0.3.5</t>
+  </si>
+  <si>
+    <t>https://github.com/karma-runner/karma-jasmine/blob/master/LICENSE</t>
+  </si>
+  <si>
+    <t>https://github.com/karma-runner/karma-jasmine</t>
+  </si>
+  <si>
+    <t>Karma-Junit-Reporter</t>
+  </si>
+  <si>
+    <t>0.2.2</t>
+  </si>
+  <si>
+    <t>https://github.com/karma-runner/karma-junit-reporter/blob/master/LICENSE</t>
+  </si>
+  <si>
+    <t>https://github.com/karma-runner/karma-junit-reporter</t>
+  </si>
+  <si>
+    <t>Karma-Chrome-Launcher</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>https://github.com/karma-runner/karma-chrome-launcher/blob/master/LICENSE</t>
+  </si>
+  <si>
+    <t>https://github.com/karma-runner/karma-chrome-launcher</t>
+  </si>
+  <si>
+    <t>Starts Google Chrome</t>
   </si>
 </sst>
 </file>
@@ -338,8 +404,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table167" displayName="Table167" ref="A1:K24" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table167" displayName="Table167" ref="A1:K29" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K29"/>
   <sortState ref="A2:M74">
     <sortCondition ref="A1:A81"/>
   </sortState>
@@ -647,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,6 +1012,106 @@
         <v>68</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -956,6 +1122,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F38BE9C869A7742B4F5DC1E261FF831" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c81a3dd503577bf2e55e1cf5f361d623">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -1069,33 +1250,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7617F739-067F-4308-8E8E-D48E97AC6C80}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BAEFC8-5E64-4DBE-91A8-1626A5AF5EB9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1116,9 +1274,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BAEFC8-5E64-4DBE-91A8-1626A5AF5EB9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7617F739-067F-4308-8E8E-D48E97AC6C80}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated list and About display
</commit_message>
<xml_diff>
--- a/docs/Software Development/NGC_ADS_Software_Baseline.xlsx
+++ b/docs/Software Development/NGC_ADS_Software_Baseline.xlsx
@@ -49,9 +49,6 @@
     <t>Modified</t>
   </si>
   <si>
-    <t>Twitter Bootstrap</t>
-  </si>
-  <si>
     <t>3.2.0</t>
   </si>
   <si>
@@ -302,6 +299,9 @@
   </si>
   <si>
     <t>Starts Google Chrome</t>
+  </si>
+  <si>
+    <t>Bootstrap</t>
   </si>
 </sst>
 </file>
@@ -716,7 +716,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,342 +774,342 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
         <v>58</v>
       </c>
-      <c r="D9" t="s">
-        <v>59</v>
-      </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1122,21 +1122,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F38BE9C869A7742B4F5DC1E261FF831" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c81a3dd503577bf2e55e1cf5f361d623">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -1250,10 +1235,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BAEFC8-5E64-4DBE-91A8-1626A5AF5EB9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7617F739-067F-4308-8E8E-D48E97AC6C80}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1274,17 +1282,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7617F739-067F-4308-8E8E-D48E97AC6C80}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BAEFC8-5E64-4DBE-91A8-1626A5AF5EB9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added MonogoDB to software list
</commit_message>
<xml_diff>
--- a/docs/Software Development/NGC_ADS_Software_Baseline.xlsx
+++ b/docs/Software Development/NGC_ADS_Software_Baseline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
   <si>
     <t>Product</t>
   </si>
@@ -302,6 +302,24 @@
   </si>
   <si>
     <t>Bootstrap</t>
+  </si>
+  <si>
+    <t>MongoDB</t>
+  </si>
+  <si>
+    <t>https://www.mongodb.org/about/licensing/</t>
+  </si>
+  <si>
+    <t>3.0.4</t>
+  </si>
+  <si>
+    <t>https://www.mongodb.org/</t>
+  </si>
+  <si>
+    <t>Caching</t>
+  </si>
+  <si>
+    <t>GNU Affero General Public License Version 3.0</t>
   </si>
 </sst>
 </file>
@@ -713,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,6 +1130,26 @@
         <v>94</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -1122,6 +1160,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F38BE9C869A7742B4F5DC1E261FF831" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c81a3dd503577bf2e55e1cf5f361d623">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -1235,33 +1288,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7617F739-067F-4308-8E8E-D48E97AC6C80}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BAEFC8-5E64-4DBE-91A8-1626A5AF5EB9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1282,9 +1312,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BAEFC8-5E64-4DBE-91A8-1626A5AF5EB9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7617F739-067F-4308-8E8E-D48E97AC6C80}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated open source list
</commit_message>
<xml_diff>
--- a/docs/Software Development/NGC_ADS_Software_Baseline.xlsx
+++ b/docs/Software Development/NGC_ADS_Software_Baseline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="111">
   <si>
     <t>Product</t>
   </si>
@@ -329,6 +329,24 @@
   </si>
   <si>
     <t>3.9.3</t>
+  </si>
+  <si>
+    <t>UnitJS</t>
+  </si>
+  <si>
+    <t>Mocha</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/unit.js</t>
+  </si>
+  <si>
+    <t>2.0.0</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/mocha</t>
+  </si>
+  <si>
+    <t>2.2.5</t>
   </si>
 </sst>
 </file>
@@ -740,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,6 +1197,46 @@
         <v>55</v>
       </c>
     </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
@@ -1189,21 +1247,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F38BE9C869A7742B4F5DC1E261FF831" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c81a3dd503577bf2e55e1cf5f361d623">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -1317,10 +1360,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BAEFC8-5E64-4DBE-91A8-1626A5AF5EB9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7617F739-067F-4308-8E8E-D48E97AC6C80}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1341,17 +1407,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7617F739-067F-4308-8E8E-D48E97AC6C80}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BAEFC8-5E64-4DBE-91A8-1626A5AF5EB9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>